<commit_message>
Atualização de todos os arquivos que foram modificados no repositório da faculdade
</commit_message>
<xml_diff>
--- a/TI-Aula5-Backlog-Grupo02.xlsx
+++ b/TI-Aula5-Backlog-Grupo02.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/mateus_nascimento_bandtec_com_br/Documents/BandTec01/Tecnologia da informação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91d76e36d2298fec/Área de Trabalho/P.I/projetos/grupo02-1adsa-2021-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="14_{3F79D825-B184-401A-8EF5-9A5D9F08C9E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EFAD01A8-A3E8-4524-94F8-C5CC5C5C9931}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="14_{3F79D825-B184-401A-8EF5-9A5D9F08C9E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F6820CE9-CDAB-4627-AC69-41269A8779E0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3E66C769-B42B-472F-8C84-909496EE0B94}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Nome do requisito</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Atividade No. 05 - CLASSIFICAÇÃO BACKLOG</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
   </si>
 </sst>
 </file>
@@ -226,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,44 +244,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -594,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A0C09D-E627-4D34-A96C-4DD9B25C29FE}">
-  <dimension ref="B2:J29"/>
+  <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C19" sqref="C19:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,375 +614,393 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="10">
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12">
         <v>1</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10">
+      <c r="H5" s="13"/>
+      <c r="I5" s="12">
         <v>21</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="10">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12">
         <v>2</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="10">
+      <c r="H6" s="13"/>
+      <c r="I6" s="12">
         <v>3</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="10">
+      <c r="D7" s="9"/>
+      <c r="E7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12">
         <v>3</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10">
+      <c r="H7" s="13"/>
+      <c r="I7" s="12">
         <v>3</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="10">
+      <c r="D8" s="9"/>
+      <c r="E8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12">
         <v>4</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10">
-        <v>5</v>
-      </c>
-      <c r="J8" s="11"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="12">
+        <v>5</v>
+      </c>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="10">
-        <v>5</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="10">
-        <v>5</v>
-      </c>
-      <c r="J9" s="11"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12">
+        <v>5</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="12">
+        <v>5</v>
+      </c>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="10">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12">
         <v>6</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="10">
-        <v>5</v>
-      </c>
-      <c r="J10" s="11"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="12">
+        <v>5</v>
+      </c>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="10">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12">
         <v>7</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10">
+      <c r="H11" s="13"/>
+      <c r="I11" s="12">
         <v>13</v>
       </c>
-      <c r="J11" s="11"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="10">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12">
         <v>8</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="10">
+      <c r="H12" s="13"/>
+      <c r="I12" s="12">
         <v>13</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="10">
+      <c r="F13" s="11"/>
+      <c r="G13" s="12">
         <v>9</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10">
-        <v>5</v>
-      </c>
-      <c r="J13" s="11"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="12">
+        <v>5</v>
+      </c>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="12" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="10">
+      <c r="F14" s="11"/>
+      <c r="G14" s="12">
         <v>10</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="10">
+      <c r="H14" s="13"/>
+      <c r="I14" s="12">
         <v>13</v>
       </c>
-      <c r="J14" s="11"/>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="12" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="10">
+      <c r="F15" s="11"/>
+      <c r="G15" s="12">
         <v>11</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="10">
-        <v>5</v>
-      </c>
-      <c r="J15" s="11"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="12">
+        <v>5</v>
+      </c>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="12" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="10">
+      <c r="F16" s="11"/>
+      <c r="G16" s="12">
         <v>12</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="10">
-        <v>5</v>
-      </c>
-      <c r="J16" s="11"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="12">
+        <v>5</v>
+      </c>
+      <c r="J16" s="13"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="12" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="10">
+      <c r="F17" s="11"/>
+      <c r="G17" s="12">
         <v>13</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="10">
+      <c r="H17" s="13"/>
+      <c r="I17" s="12">
         <v>13</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="13"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="10">
+      <c r="F18" s="11"/>
+      <c r="G18" s="12">
         <v>14</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="10">
+      <c r="H18" s="13"/>
+      <c r="I18" s="12">
         <v>8</v>
       </c>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="2" t="s">
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16">
+        <v>15</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16">
+        <v>13</v>
+      </c>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="4" t="s">
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="C27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="E4:J18" xr:uid="{7085D056-994B-4822-9AFD-4BA201EBAE43}">
@@ -984,7 +1008,59 @@
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
-  <mergeCells count="64">
+  <mergeCells count="68">
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
@@ -1001,54 +1077,6 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>